<commit_message>
94 member csv file regenerated for better distribution
</commit_message>
<xml_diff>
--- a/mira/mira_members94.xlsx
+++ b/mira/mira_members94.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kale/Desktop/vivo/mira/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CDAB34D-D460-414F-9DD5-DD5D5BCDE32D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9211A0-2246-7C4F-9784-D7A3556C5809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26660" windowHeight="14760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4490,11 +4490,11 @@
       </c>
       <c r="H2">
         <f t="shared" ref="H2:I21" ca="1" si="0">RANDBETWEEN(0, 200)</f>
-        <v>163</v>
+        <v>25</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4518,11 +4518,11 @@
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>189</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4546,11 +4546,11 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4574,11 +4574,11 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4602,11 +4602,11 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>198</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -4630,11 +4630,11 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -4658,11 +4658,11 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -4686,11 +4686,11 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -4714,11 +4714,11 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -4742,11 +4742,11 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>121</v>
+        <v>11</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>199</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -4770,11 +4770,11 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -4798,11 +4798,11 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -4826,11 +4826,11 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>104</v>
+        <v>193</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -4854,11 +4854,11 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>193</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -4882,11 +4882,11 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -4910,11 +4910,11 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>57</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -4966,11 +4966,11 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="0"/>
-        <v>129</v>
+        <v>33</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -4994,11 +4994,11 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="0"/>
-        <v>138</v>
+        <v>64</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
-        <v>165</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -5022,11 +5022,11 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>87</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="0"/>
-        <v>188</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -5050,11 +5050,11 @@
       </c>
       <c r="H22">
         <f t="shared" ref="H22:I41" ca="1" si="1">RANDBETWEEN(0, 200)</f>
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>102</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -5078,11 +5078,11 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>183</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -5106,11 +5106,11 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>132</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -5134,11 +5134,11 @@
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -5162,11 +5162,11 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
-        <v>115</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -5190,11 +5190,11 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>194</v>
+        <v>4</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -5218,11 +5218,11 @@
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
-        <v>125</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -5246,11 +5246,11 @@
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -5274,11 +5274,11 @@
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="1"/>
-        <v>113</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -5302,11 +5302,11 @@
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>158</v>
+        <v>199</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="1"/>
-        <v>114</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -5330,11 +5330,11 @@
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -5358,11 +5358,11 @@
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>198</v>
+        <v>128</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="1"/>
-        <v>168</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -5386,11 +5386,11 @@
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -5414,11 +5414,11 @@
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>172</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="1"/>
-        <v>169</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -5442,11 +5442,11 @@
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="1"/>
-        <v>142</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -5470,11 +5470,11 @@
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -5498,11 +5498,11 @@
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="1"/>
-        <v>161</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -5526,11 +5526,11 @@
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>135</v>
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="1"/>
-        <v>132</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -5554,11 +5554,11 @@
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="1"/>
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -5582,11 +5582,11 @@
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="1"/>
-        <v>158</v>
+        <v>41</v>
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="1"/>
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -5610,11 +5610,11 @@
       </c>
       <c r="H42">
         <f t="shared" ref="H42:I61" ca="1" si="2">RANDBETWEEN(0, 200)</f>
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="2"/>
-        <v>182</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -5638,11 +5638,11 @@
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="2"/>
-        <v>153</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -5666,11 +5666,11 @@
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="2"/>
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="2"/>
-        <v>123</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -5694,11 +5694,11 @@
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="2"/>
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -5722,11 +5722,11 @@
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="2"/>
-        <v>115</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -5750,11 +5750,11 @@
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="2"/>
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="2"/>
-        <v>190</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -5778,11 +5778,11 @@
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="2"/>
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -5806,11 +5806,11 @@
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="2"/>
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="2"/>
-        <v>184</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -5834,11 +5834,11 @@
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="2"/>
-        <v>52</v>
+        <v>139</v>
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="2"/>
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -5862,11 +5862,11 @@
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="2"/>
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -5890,11 +5890,11 @@
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="2"/>
-        <v>128</v>
+        <v>58</v>
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="2"/>
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -5918,11 +5918,11 @@
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="2"/>
-        <v>102</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -5946,11 +5946,11 @@
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="2"/>
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="2"/>
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -5974,11 +5974,11 @@
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="2"/>
-        <v>37</v>
+        <v>192</v>
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="2"/>
-        <v>55</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -6002,11 +6002,11 @@
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="2"/>
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="2"/>
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -6030,11 +6030,11 @@
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="2"/>
-        <v>129</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -6058,11 +6058,11 @@
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="2"/>
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="2"/>
-        <v>121</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -6086,11 +6086,11 @@
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="2"/>
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -6114,11 +6114,11 @@
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="2"/>
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="2"/>
-        <v>179</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -6142,11 +6142,11 @@
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="2"/>
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="2"/>
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -6170,11 +6170,11 @@
       </c>
       <c r="H62">
         <f t="shared" ref="H62:I81" ca="1" si="3">RANDBETWEEN(0, 200)</f>
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="3"/>
-        <v>84</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -6198,11 +6198,11 @@
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>185</v>
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -6226,11 +6226,11 @@
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="3"/>
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="3"/>
-        <v>147</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -6254,11 +6254,11 @@
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="3"/>
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -6282,11 +6282,11 @@
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>164</v>
       </c>
       <c r="I66">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -6310,11 +6310,11 @@
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="3"/>
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -6338,11 +6338,11 @@
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -6366,11 +6366,11 @@
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -6394,11 +6394,11 @@
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="3"/>
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="3"/>
-        <v>197</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -6422,11 +6422,11 @@
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="3"/>
-        <v>52</v>
+        <v>169</v>
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -6450,11 +6450,11 @@
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="3"/>
-        <v>58</v>
+        <v>199</v>
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -6478,11 +6478,11 @@
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="3"/>
-        <v>173</v>
+        <v>1</v>
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="3"/>
-        <v>75</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -6506,11 +6506,11 @@
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="3"/>
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="3"/>
-        <v>151</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -6534,11 +6534,11 @@
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="3"/>
-        <v>130</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -6562,11 +6562,11 @@
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="3"/>
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="3"/>
-        <v>180</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -6590,11 +6590,11 @@
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="3"/>
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -6618,11 +6618,11 @@
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="3"/>
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="3"/>
-        <v>155</v>
+        <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -6646,11 +6646,11 @@
       </c>
       <c r="H79">
         <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -6674,11 +6674,11 @@
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="3"/>
-        <v>186</v>
+        <v>63</v>
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -6702,11 +6702,11 @@
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I81">
         <f t="shared" ca="1" si="3"/>
-        <v>152</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -6730,11 +6730,11 @@
       </c>
       <c r="H82">
         <f t="shared" ref="H82:I95" ca="1" si="4">RANDBETWEEN(0, 200)</f>
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="I82">
         <f t="shared" ca="1" si="4"/>
-        <v>145</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -6758,11 +6758,11 @@
       </c>
       <c r="H83">
         <f t="shared" ca="1" si="4"/>
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="I83">
         <f t="shared" ca="1" si="4"/>
-        <v>154</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -6786,11 +6786,11 @@
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="4"/>
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="I84">
         <f t="shared" ca="1" si="4"/>
-        <v>170</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -6814,11 +6814,11 @@
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="4"/>
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="I85">
         <f t="shared" ca="1" si="4"/>
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -6842,11 +6842,11 @@
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="4"/>
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I86">
         <f t="shared" ca="1" si="4"/>
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -6870,11 +6870,11 @@
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="4"/>
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="I87">
         <f t="shared" ca="1" si="4"/>
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
@@ -6898,11 +6898,11 @@
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="4"/>
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="I88">
         <f t="shared" ca="1" si="4"/>
-        <v>176</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
@@ -6926,11 +6926,11 @@
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>197</v>
       </c>
       <c r="I89">
         <f t="shared" ca="1" si="4"/>
-        <v>39</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
@@ -6954,11 +6954,11 @@
       </c>
       <c r="H90">
         <f t="shared" ca="1" si="4"/>
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="I90">
         <f t="shared" ca="1" si="4"/>
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -6982,11 +6982,11 @@
       </c>
       <c r="H91">
         <f t="shared" ca="1" si="4"/>
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="I91">
         <f t="shared" ca="1" si="4"/>
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -7010,11 +7010,11 @@
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="4"/>
-        <v>200</v>
+        <v>137</v>
       </c>
       <c r="I92">
         <f t="shared" ca="1" si="4"/>
-        <v>65</v>
+        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
@@ -7038,11 +7038,11 @@
       </c>
       <c r="H93">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="I93">
         <f t="shared" ca="1" si="4"/>
-        <v>169</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -7066,11 +7066,11 @@
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="4"/>
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="I94">
         <f t="shared" ca="1" si="4"/>
-        <v>100</v>
+        <v>43</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
@@ -7094,11 +7094,11 @@
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="4"/>
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="I95">
         <f t="shared" ca="1" si="4"/>
-        <v>116</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -7111,7 +7111,7 @@
   <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7170,10 +7170,10 @@
         <v>347</v>
       </c>
       <c r="H2">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="I2">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -7196,10 +7196,10 @@
         <v>347</v>
       </c>
       <c r="H3">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="I3">
-        <v>116</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -7222,10 +7222,10 @@
         <v>347</v>
       </c>
       <c r="H4">
-        <v>139</v>
+        <v>56</v>
       </c>
       <c r="I4">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -7248,10 +7248,10 @@
         <v>347</v>
       </c>
       <c r="H5">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="I5">
-        <v>197</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -7274,10 +7274,10 @@
         <v>347</v>
       </c>
       <c r="H6">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I6">
-        <v>15</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -7303,7 +7303,7 @@
         <v>18</v>
       </c>
       <c r="I7">
-        <v>125</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -7326,10 +7326,10 @@
         <v>347</v>
       </c>
       <c r="H8">
-        <v>134</v>
+        <v>97</v>
       </c>
       <c r="I8">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -7352,10 +7352,10 @@
         <v>347</v>
       </c>
       <c r="H9">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="I9">
-        <v>75</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -7378,10 +7378,10 @@
         <v>347</v>
       </c>
       <c r="H10">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="I10">
-        <v>132</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -7404,10 +7404,10 @@
         <v>347</v>
       </c>
       <c r="H11">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="I11">
-        <v>51</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -7430,10 +7430,10 @@
         <v>347</v>
       </c>
       <c r="H12">
-        <v>186</v>
+        <v>108</v>
       </c>
       <c r="I12">
-        <v>170</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -7456,10 +7456,10 @@
         <v>318</v>
       </c>
       <c r="H13">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="I13">
-        <v>44</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -7482,10 +7482,10 @@
         <v>318</v>
       </c>
       <c r="H14">
-        <v>26</v>
+        <v>172</v>
       </c>
       <c r="I14">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -7508,10 +7508,10 @@
         <v>318</v>
       </c>
       <c r="H15">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="I15">
-        <v>132</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -7534,10 +7534,10 @@
         <v>318</v>
       </c>
       <c r="H16">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="I16">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -7560,10 +7560,10 @@
         <v>318</v>
       </c>
       <c r="H17">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="I17">
-        <v>75</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -7586,10 +7586,10 @@
         <v>318</v>
       </c>
       <c r="H18">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="I18">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -7612,10 +7612,10 @@
         <v>318</v>
       </c>
       <c r="H19">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="I19">
-        <v>174</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -7638,10 +7638,10 @@
         <v>318</v>
       </c>
       <c r="H20">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="I20">
-        <v>108</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -7664,10 +7664,10 @@
         <v>318</v>
       </c>
       <c r="H21">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="I21">
-        <v>162</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -7690,10 +7690,10 @@
         <v>318</v>
       </c>
       <c r="H22">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="I22">
-        <v>15</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -7716,10 +7716,10 @@
         <v>318</v>
       </c>
       <c r="H23">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="I23">
-        <v>42</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -7742,10 +7742,10 @@
         <v>318</v>
       </c>
       <c r="H24">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -7768,10 +7768,10 @@
         <v>318</v>
       </c>
       <c r="H25">
-        <v>121</v>
+        <v>27</v>
       </c>
       <c r="I25">
-        <v>92</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -7794,10 +7794,10 @@
         <v>318</v>
       </c>
       <c r="H26">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="I26">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -7820,10 +7820,10 @@
         <v>303</v>
       </c>
       <c r="H27">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="I27">
-        <v>122</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -7846,10 +7846,10 @@
         <v>303</v>
       </c>
       <c r="H28">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="I28">
-        <v>86</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -7872,10 +7872,10 @@
         <v>303</v>
       </c>
       <c r="H29">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I29">
-        <v>153</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -7898,10 +7898,10 @@
         <v>303</v>
       </c>
       <c r="H30">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="I30">
-        <v>92</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -7924,10 +7924,10 @@
         <v>303</v>
       </c>
       <c r="H31">
-        <v>106</v>
+        <v>37</v>
       </c>
       <c r="I31">
-        <v>163</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -7950,10 +7950,10 @@
         <v>303</v>
       </c>
       <c r="H32">
-        <v>157</v>
+        <v>62</v>
       </c>
       <c r="I32">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -7976,10 +7976,10 @@
         <v>303</v>
       </c>
       <c r="H33">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="I33">
-        <v>141</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -8002,10 +8002,10 @@
         <v>303</v>
       </c>
       <c r="H34">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="I34">
-        <v>150</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -8028,10 +8028,10 @@
         <v>303</v>
       </c>
       <c r="H35">
-        <v>27</v>
+        <v>190</v>
       </c>
       <c r="I35">
-        <v>141</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -8054,10 +8054,10 @@
         <v>303</v>
       </c>
       <c r="H36">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="I36">
-        <v>11</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -8080,10 +8080,10 @@
         <v>395</v>
       </c>
       <c r="H37">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="I37">
-        <v>157</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -8106,10 +8106,10 @@
         <v>395</v>
       </c>
       <c r="H38">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="I38">
-        <v>177</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -8132,10 +8132,10 @@
         <v>395</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>185</v>
       </c>
       <c r="I39">
-        <v>199</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -8158,10 +8158,10 @@
         <v>395</v>
       </c>
       <c r="H40">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="I40">
-        <v>194</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -8184,10 +8184,10 @@
         <v>395</v>
       </c>
       <c r="H41">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I41">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -8210,10 +8210,10 @@
         <v>395</v>
       </c>
       <c r="H42">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="I42">
-        <v>45</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -8239,7 +8239,7 @@
         <v>158</v>
       </c>
       <c r="I43">
-        <v>106</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -8262,10 +8262,10 @@
         <v>395</v>
       </c>
       <c r="H44">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="I44">
-        <v>129</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -8288,10 +8288,10 @@
         <v>395</v>
       </c>
       <c r="H45">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="I45">
-        <v>24</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -8314,10 +8314,10 @@
         <v>395</v>
       </c>
       <c r="H46">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="I46">
-        <v>86</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -8340,10 +8340,10 @@
         <v>395</v>
       </c>
       <c r="H47">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="I47">
-        <v>91</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -8366,10 +8366,10 @@
         <v>395</v>
       </c>
       <c r="H48">
-        <v>189</v>
+        <v>62</v>
       </c>
       <c r="I48">
-        <v>184</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -8392,10 +8392,10 @@
         <v>362</v>
       </c>
       <c r="H49">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="I49">
-        <v>5</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -8418,10 +8418,10 @@
         <v>362</v>
       </c>
       <c r="H50">
-        <v>163</v>
+        <v>94</v>
       </c>
       <c r="I50">
-        <v>159</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -8444,10 +8444,10 @@
         <v>362</v>
       </c>
       <c r="H51">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I51">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -8470,10 +8470,10 @@
         <v>362</v>
       </c>
       <c r="H52">
-        <v>169</v>
+        <v>74</v>
       </c>
       <c r="I52">
-        <v>68</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -8496,10 +8496,10 @@
         <v>362</v>
       </c>
       <c r="H53">
-        <v>128</v>
+        <v>43</v>
       </c>
       <c r="I53">
-        <v>41</v>
+        <v>184</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -8522,10 +8522,10 @@
         <v>362</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="I54">
-        <v>35</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -8548,10 +8548,10 @@
         <v>362</v>
       </c>
       <c r="H55">
-        <v>83</v>
+        <v>164</v>
       </c>
       <c r="I55">
-        <v>189</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -8574,10 +8574,10 @@
         <v>362</v>
       </c>
       <c r="H56">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="I56">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -8600,10 +8600,10 @@
         <v>362</v>
       </c>
       <c r="H57">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="I57">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -8626,10 +8626,10 @@
         <v>362</v>
       </c>
       <c r="H58">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I58">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -8652,10 +8652,10 @@
         <v>362</v>
       </c>
       <c r="H59">
-        <v>43</v>
+        <v>196</v>
       </c>
       <c r="I59">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -8678,10 +8678,10 @@
         <v>362</v>
       </c>
       <c r="H60">
-        <v>183</v>
+        <v>74</v>
       </c>
       <c r="I60">
-        <v>151</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -8704,10 +8704,10 @@
         <v>362</v>
       </c>
       <c r="H61">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="I61">
-        <v>30</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -8730,10 +8730,10 @@
         <v>362</v>
       </c>
       <c r="H62">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="I62">
-        <v>170</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -8756,7 +8756,7 @@
         <v>362</v>
       </c>
       <c r="H63">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="I63">
         <v>29</v>
@@ -8782,10 +8782,10 @@
         <v>362</v>
       </c>
       <c r="H64">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="I64">
-        <v>117</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -8808,10 +8808,10 @@
         <v>347</v>
       </c>
       <c r="H65">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I65">
-        <v>180</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -8834,10 +8834,10 @@
         <v>347</v>
       </c>
       <c r="H66">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="I66">
-        <v>137</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -8860,10 +8860,10 @@
         <v>347</v>
       </c>
       <c r="H67">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="I67">
-        <v>33</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -8886,10 +8886,10 @@
         <v>347</v>
       </c>
       <c r="H68">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="I68">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -8912,10 +8912,10 @@
         <v>347</v>
       </c>
       <c r="H69">
-        <v>77</v>
+        <v>138</v>
       </c>
       <c r="I69">
-        <v>56</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -8938,10 +8938,10 @@
         <v>347</v>
       </c>
       <c r="H70">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="I70">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -8964,10 +8964,10 @@
         <v>347</v>
       </c>
       <c r="H71">
-        <v>12</v>
+        <v>140</v>
       </c>
       <c r="I71">
-        <v>117</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -8990,10 +8990,10 @@
         <v>318</v>
       </c>
       <c r="H72">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="I72">
-        <v>83</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -9016,10 +9016,10 @@
         <v>318</v>
       </c>
       <c r="H73">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="I73">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -9042,10 +9042,10 @@
         <v>318</v>
       </c>
       <c r="H74">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="I74">
-        <v>82</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -9068,10 +9068,10 @@
         <v>318</v>
       </c>
       <c r="H75">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I75">
-        <v>170</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -9094,10 +9094,10 @@
         <v>318</v>
       </c>
       <c r="H76">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="I76">
-        <v>99</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -9120,10 +9120,10 @@
         <v>318</v>
       </c>
       <c r="H77">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I77">
-        <v>183</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -9146,10 +9146,10 @@
         <v>318</v>
       </c>
       <c r="H78">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="I78">
-        <v>189</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -9172,10 +9172,10 @@
         <v>318</v>
       </c>
       <c r="H79">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="I79">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -9198,10 +9198,10 @@
         <v>318</v>
       </c>
       <c r="H80">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="I80">
-        <v>143</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -9224,10 +9224,10 @@
         <v>318</v>
       </c>
       <c r="H81">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="I81">
-        <v>94</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -9250,10 +9250,10 @@
         <v>318</v>
       </c>
       <c r="H82">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="I82">
-        <v>58</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -9276,10 +9276,10 @@
         <v>318</v>
       </c>
       <c r="H83">
-        <v>24</v>
+        <v>182</v>
       </c>
       <c r="I83">
-        <v>15</v>
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -9302,10 +9302,10 @@
         <v>318</v>
       </c>
       <c r="H84">
-        <v>164</v>
+        <v>2</v>
       </c>
       <c r="I84">
-        <v>191</v>
+        <v>92</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -9328,10 +9328,10 @@
         <v>318</v>
       </c>
       <c r="H85">
-        <v>178</v>
+        <v>42</v>
       </c>
       <c r="I85">
-        <v>130</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -9354,10 +9354,10 @@
         <v>303</v>
       </c>
       <c r="H86">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="I86">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -9380,10 +9380,10 @@
         <v>303</v>
       </c>
       <c r="H87">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="I87">
-        <v>41</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
@@ -9406,10 +9406,10 @@
         <v>303</v>
       </c>
       <c r="H88">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="I88">
-        <v>148</v>
+        <v>174</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
@@ -9432,10 +9432,10 @@
         <v>303</v>
       </c>
       <c r="H89">
-        <v>165</v>
+        <v>78</v>
       </c>
       <c r="I89">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
@@ -9458,10 +9458,10 @@
         <v>303</v>
       </c>
       <c r="H90">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="I90">
-        <v>7</v>
+        <v>192</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -9484,10 +9484,10 @@
         <v>303</v>
       </c>
       <c r="H91">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="I91">
-        <v>130</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -9510,10 +9510,10 @@
         <v>303</v>
       </c>
       <c r="H92">
-        <v>148</v>
+        <v>55</v>
       </c>
       <c r="I92">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
@@ -9536,10 +9536,10 @@
         <v>295</v>
       </c>
       <c r="H93">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="I93">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -9562,10 +9562,10 @@
         <v>295</v>
       </c>
       <c r="H94">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="I94">
-        <v>125</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
@@ -9588,10 +9588,10 @@
         <v>295</v>
       </c>
       <c r="H95">
-        <v>154</v>
+        <v>27</v>
       </c>
       <c r="I95">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>